<commit_message>
Data update, added polygons (first datapoint) from xml source
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G2" s="12" t="n">
         <v>110</v>
@@ -788,8 +788,8 @@
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>"place = town", 40
-"source:population = SSB - befolkning i tettstedet", 48
+          <t>"place = town", 42
+"source:population = SSB - befolkning i tettstedet", 50
 "place = city", 14
 "ref:ssb_tettsted = 2562", 2
 "ref:ssb_tettsted = 2511", 2
@@ -804,9 +804,11 @@
 "ref:ssb_tettsted = 3021", 2
 "ref:ssb_tettsted = 3005-3813", 2
 "ref:ssb_tettsted = 3054", 2
+"ref:ssb_tettsted = 3102", 2
 "ref:ssb_tettsted = 3501", 2
 "email = postmottak@kristiansand.kommune.no", 2
 "ref:ssb_tettsted = 4002", 2
+"ref:ssb_tettsted = 4011", 2
 "ref:ssb_tettsted = 3531", 2
 "ref:ssb_tettsted = 4091", 2</t>
         </is>
@@ -850,7 +852,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>895</v>
+        <v>874</v>
       </c>
       <c r="G3" s="12" t="n">
         <v>866</v>
@@ -873,12 +875,12 @@
       <c r="K3" s="1" t="inlineStr">
         <is>
           <t>"place = village", 199
-"source:population = SSB - befolkning i tettstedet", 129
+"source:population = SSB - befolkning i tettstedet", 130
 "place = town", 11
-"place = suburb", 43
-"place = hamlet", 17
+"place = suburb", 46
+"place = hamlet", 15
 "place = quarter", 25
-"place = neighbourhood", 20
+"place = neighbourhood", 19
 "type = multipolygon", 9</t>
         </is>
       </c>
@@ -915,7 +917,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1002</v>
+        <v>1020</v>
       </c>
       <c r="G4" s="12" t="n">
         <v>845</v>
@@ -937,11 +939,11 @@
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>"place = village", 83
+          <t>"place = village", 84
 "source:population = SSB - befolkning i tettstedet", 41
 "place = neighbourhood", 186
-"place = suburb", 91
-"place = hamlet", 49
+"place = suburb", 94
+"place = hamlet", 48
 "place = quarter", 64</t>
         </is>
       </c>
@@ -989,7 +991,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1964</v>
+        <v>1948</v>
       </c>
       <c r="G5" s="12" t="n">
         <v>2132</v>
@@ -1011,11 +1013,11 @@
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>"place = village", 224
-"place = hamlet", 158
+          <t>"place = village", 227
+"place = hamlet", 163
 "place = suburb", 19
-"source:population = SSB - befolkning i tettstedet", 30
-"place = neighbourhood", 17</t>
+"source:population = SSB - befolkning i tettstedet", 29
+"place = neighbourhood", 16</t>
         </is>
       </c>
       <c r="L5" s="17" t="inlineStr">
@@ -1061,7 +1063,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3216</v>
+        <v>3254</v>
       </c>
       <c r="G6" s="12" t="n">
         <v>3300</v>
@@ -1083,10 +1085,10 @@
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>"place = hamlet", 738
-"place = neighbourhood", 60
-"place = farm", 39
-"place = village", 36</t>
+          <t>"place = hamlet", 787
+"place = neighbourhood", 64
+"place = farm", 42
+"place = village", 37</t>
         </is>
       </c>
       <c r="L6" s="17" t="inlineStr">
@@ -1122,7 +1124,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2801</v>
+        <v>2849</v>
       </c>
       <c r="G7" s="12" t="n">
         <v>2027</v>
@@ -1144,7 +1146,7 @@
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>"place = neighbourhood", 775
+          <t>"place = neighbourhood", 798
 "landuse = residential", 31
 "place = suburb", 49
 "place = quarter", 202</t>
@@ -1183,7 +1185,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="G8" s="12" t="n">
         <v>372</v>
@@ -1205,15 +1207,16 @@
       </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>"landuse = industrial", 48
-"type = multipolygon", 11
+          <t>"landuse = industrial", 49
+"type = multipolygon", 12
 "place = quarter", 21
 "place = locality", 26
 "place = suburb", 7
 "natural = cape", 2
 "building = industrial", 4
 "man_made = wastewater_plant", 2
-"place = neighbourhood", 40
+"place = neighbourhood", 42
+"place = farm", 2
 "place = isolated_dwelling", 2
 "ref:bygningsnr = 166261902", 2
 "landuse = retail", 2</t>
@@ -1252,7 +1255,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>416</v>
+        <v>448</v>
       </c>
       <c r="G9" s="12" t="n">
         <v>395</v>
@@ -1274,8 +1277,8 @@
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>"place = suburb", 109
-"place = neighbourhood", 13
+          <t>"place = suburb", 118
+"place = neighbourhood", 14
 "place = quarter", 21
 "place = village", 4</t>
         </is>
@@ -1313,7 +1316,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>857</v>
+        <v>878</v>
       </c>
       <c r="G10" s="12" t="n">
         <v>536</v>
@@ -1335,7 +1338,7 @@
       </c>
       <c r="K10" s="1" t="inlineStr">
         <is>
-          <t>"place = neighbourhood", 181
+          <t>"place = neighbourhood", 184
 "place = quarter", 9
 "landuse = residential", 10</t>
         </is>
@@ -1373,7 +1376,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="G11" s="12" t="n">
         <v>112</v>
@@ -1395,7 +1398,7 @@
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>"place = square", 42</t>
+          <t>"place = square", 44</t>
         </is>
       </c>
       <c r="L11" s="17" t="inlineStr">
@@ -1431,7 +1434,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" s="12" t="n">
         <v>59</v>
@@ -1545,7 +1548,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
@@ -1556,7 +1559,7 @@
       <c r="K14" s="1" t="inlineStr">
         <is>
           <t>"place = locality", 3
-"place = isolated_dwelling", 2</t>
+"place = isolated_dwelling", 3</t>
         </is>
       </c>
       <c r="M14" s="12" t="inlineStr">
@@ -1592,7 +1595,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G15" s="12" t="n">
         <v>19</v>
@@ -1650,7 +1653,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>10186</v>
+        <v>9734</v>
       </c>
       <c r="G16" s="12" t="n">
         <v>11736</v>
@@ -1672,8 +1675,8 @@
       </c>
       <c r="K16" s="1" t="inlineStr">
         <is>
-          <t>"place = isolated_dwelling", 3195
-"place = farm", 533</t>
+          <t>"place = isolated_dwelling", 3011
+"place = farm", 537</t>
         </is>
       </c>
       <c r="L16" s="2" t="inlineStr">
@@ -1714,7 +1717,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>13842</v>
+        <v>13462</v>
       </c>
       <c r="G17" s="12" t="n">
         <v>13094</v>
@@ -1736,10 +1739,10 @@
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>"building = cabin", 943
-"place = isolated_dwelling", 5380
-"place = locality", 350
-"historic = shieling", 685</t>
+          <t>"building = cabin", 1018
+"place = isolated_dwelling", 5640
+"place = locality", 362
+"historic = shieling", 734</t>
         </is>
       </c>
       <c r="L17" s="2" t="inlineStr">
@@ -1775,7 +1778,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>10582</v>
+        <v>11043</v>
       </c>
       <c r="G18" s="12" t="n">
         <v>6992</v>
@@ -1797,9 +1800,9 @@
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 5711
-"historic = shieling", 1020
-"historic = ruins", 836</t>
+          <t>"place = locality", 6075
+"historic = shieling", 1090
+"historic = ruins", 844</t>
         </is>
       </c>
       <c r="L18" s="2" t="n"/>
@@ -1901,7 +1904,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="G20" s="12" t="n">
         <v>131</v>
@@ -1961,7 +1964,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="G21" s="12" t="n">
         <v>80</v>
@@ -2026,7 +2029,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>717</v>
+        <v>771</v>
       </c>
       <c r="G22" s="12" t="n">
         <v>513</v>
@@ -2048,11 +2051,11 @@
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>"leisure = pitch", 75
-"sport = soccer", 32
+          <t>"leisure = pitch", 77
+"sport = soccer", 34
 "type = multipolygon", 7
 "sport = horse_racing", 6
-"place = locality", 17
+"place = locality", 19
 "leisure = sports_centre", 10
 "surface = grass", 5
 "leisure = track", 3
@@ -2092,7 +2095,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G23" s="12" t="n">
         <v>24</v>
@@ -2211,7 +2214,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G25" s="12" t="n">
         <v>45</v>
@@ -2234,10 +2237,11 @@
       <c r="K25" s="1" t="inlineStr">
         <is>
           <t>"leisure = swimming_area", 20
-"place = locality", 24
-"natural = beach", 10
-"surface = sand", 10
-"layer = 2", 3</t>
+"place = locality", 25
+"natural = beach", 13
+"surface = sand", 13
+"layer = 2", 6
+"description:no = Stranda har fått navnet sitt etter den rødfarget sanden, denne rødfargen stammer fra ned rustet tyskt materiell som ble ligende her etter 2. verdenskrig, som nettopp minner om kanelfarge.", 2</t>
         </is>
       </c>
       <c r="L25" s="17" t="inlineStr">
@@ -2338,7 +2342,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>100683</v>
+        <v>100385</v>
       </c>
       <c r="G27" s="12" t="n">
         <v>117578</v>
@@ -2360,7 +2364,7 @@
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>"place = farm", 28741</t>
+          <t>"place = farm", 29422</t>
         </is>
       </c>
       <c r="L27" s="17" t="inlineStr">
@@ -2401,7 +2405,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>21910</v>
+        <v>21534</v>
       </c>
       <c r="G28" s="12" t="n">
         <v>18129</v>
@@ -2423,9 +2427,9 @@
       </c>
       <c r="K28" s="1" t="inlineStr">
         <is>
-          <t>"historic = shieling", 6379
-"place = locality", 5246
-"place = isolated_dwelling", 1171</t>
+          <t>"historic = shieling", 6820
+"place = locality", 5687
+"place = isolated_dwelling", 1174</t>
         </is>
       </c>
       <c r="L28" s="17" t="inlineStr">
@@ -2466,7 +2470,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2566</v>
+        <v>2524</v>
       </c>
       <c r="G29" s="12" t="n">
         <v>3963</v>
@@ -2489,8 +2493,8 @@
       <c r="K29" s="1" t="inlineStr">
         <is>
           <t>"building = farm_auxiliary", 209
-"place = locality", 1120
-"historic = shieling", 179</t>
+"place = locality", 1170
+"historic = shieling", 180</t>
         </is>
       </c>
       <c r="M29" s="12" t="inlineStr">
@@ -2526,7 +2530,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>4073</v>
+        <v>4078</v>
       </c>
       <c r="G30" s="12" t="n">
         <v>2651</v>
@@ -2548,10 +2552,10 @@
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 987
-"place = farm", 181
+          <t>"place = locality", 990
+"place = farm", 200
 "place = isolated_dwelling", 55
-"historic = shieling", 53</t>
+"historic = shieling", 54</t>
         </is>
       </c>
       <c r="M30" s="17" t="inlineStr">
@@ -2587,7 +2591,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G31" s="12" t="n">
         <v>80</v>
@@ -2646,7 +2650,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>39564</v>
+        <v>39686</v>
       </c>
       <c r="G32" s="12" t="n">
         <v>3119</v>
@@ -2668,8 +2672,8 @@
       </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>"place = farm", 10573
-"place = hamlet", 1954</t>
+          <t>"place = farm", 11025
+"place = hamlet", 2053</t>
         </is>
       </c>
       <c r="L32" s="17" t="inlineStr">
@@ -2715,7 +2719,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>3257</v>
+        <v>3354</v>
       </c>
       <c r="G33" s="12" t="n">
         <v>97</v>
@@ -2737,8 +2741,8 @@
       </c>
       <c r="K33" s="1" t="inlineStr">
         <is>
-          <t>"place = farm", 329
-"place = hamlet", 566</t>
+          <t>"place = farm", 330
+"place = hamlet", 584</t>
         </is>
       </c>
       <c r="L33" s="17" t="inlineStr">
@@ -2853,7 +2857,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2121</v>
+        <v>2187</v>
       </c>
       <c r="G36" s="12" t="n">
         <v>1732</v>
@@ -2876,21 +2880,21 @@
       <c r="K36" s="1" t="inlineStr">
         <is>
           <t>"building = school", 27
-"amenity = school", 178
-"fee = no", 135
-"grades = 1-7", 67
-"isced:level = 1", 72
-"operator:type = public", 135
+"amenity = school", 181
+"fee = no", 138
+"grades = 1-7", 68
+"isced:level = 1", 74
+"operator:type = public", 138
 "grades = 1-10", 28
 "isced:level = 1;2", 37
-"place = locality", 48
+"place = locality", 49
 "was:amenity = school", 7
-"grades = 8-10", 18
-"isced:level = 2", 18
-"building = civic", 29
+"grades = 8-10", 19
+"isced:level = 2", 19
+"building = civic", 30
 "fee = yes", 13
 "operator:type = private", 13
-"building = house", 10
+"building = house", 12
 "building = kindergarten", 12
 "grades = 11-13", 21
 "isced:level = 3", 21
@@ -2930,7 +2934,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G37" s="12" t="n">
         <v>88</v>
@@ -2990,7 +2994,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="G38" s="12" t="n">
         <v>342</v>
@@ -3012,7 +3016,7 @@
       </c>
       <c r="K38" s="1" t="inlineStr">
         <is>
-          <t>"amenity = nursing_home", 81
+          <t>"amenity = nursing_home", 82
 "place = locality", 7
 "amenity = social_facility", 3
 "building = yes", 3
@@ -3052,7 +3056,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G39" s="12" t="n">
         <v>55</v>
@@ -3113,7 +3117,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G40" s="12" t="n">
         <v>67</v>
@@ -3174,7 +3178,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="G41" s="12" t="n">
         <v>251</v>
@@ -3196,7 +3200,7 @@
       </c>
       <c r="K41" s="1" t="inlineStr">
         <is>
-          <t>"amenity = kindergarten", 5
+          <t>"amenity = kindergarten", 6
 "capacity = 59", 2
 "max_age = 5", 4
 "min_age = 1", 4
@@ -3305,7 +3309,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G43" s="12" t="n">
         <v>28</v>
@@ -3419,7 +3423,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G45" s="12" t="n">
         <v>1</v>
@@ -3473,7 +3477,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G46" s="12" t="n">
         <v>367</v>
@@ -3497,7 +3501,7 @@
         <is>
           <t>"industrial = factory", 53
 "building = industrial", 40
-"place = locality", 25
+"place = locality", 26
 "type = multipolygon", 5
 "landuse = industrial", 17
 "place = neighbourhood", 10
@@ -3574,21 +3578,25 @@
       </c>
       <c r="K47" s="1" t="inlineStr">
         <is>
-          <t>"building = industrial", 60
+          <t>"building = industrial", 64
 "place = isolated_dwelling", 2
 "ref:bygningsnr = 157524291", 2
 "ref:bygningsnr = 157502042", 2
 "ref:bygningsnr = 157458736", 2
-"place = locality", 19
+"place = locality", 20
 "ref:bygningsnr = 8451478", 2
 "ref:bygningsnr = 8560013", 2
 "ref:bygningsnr = 165283686", 2
 "ref:bygningsnr = 17711024", 2
 "ref:bygningsnr = 165495055", 2
+"building = shed", 2
+"ref:bygningsnr = 165508807", 2
 "ref:bygningsnr = 8612730", 2
 "ref:bygningsnr = 165783034", 2
 "ref:bygningsnr = 165781120", 2
 "ref:bygningsnr = 165771508", 2
+"ref:bygningsnr = 165894626", 2
+"ref:bygningsnr = 165921429", 2
 "building = yes", 2
 "ref:bygningsnr = 166020549", 2
 "place = neighbourhood", 4
@@ -3638,7 +3646,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="G48" s="12" t="n">
         <v>198</v>
@@ -3713,7 +3721,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="G49" s="12" t="n">
         <v>302</v>
@@ -3738,6 +3746,7 @@
           <t>"tourism = hotel", 17
 "building = hotel", 11
 "place = locality", 11
+"tourism = chalet", 2
 "ref:bygningsnr = 8667314", 2
 "tourism = apartment", 2
 "ref:bygningsnr = 166214432", 2</t>
@@ -3776,7 +3785,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G50" s="12" t="n">
         <v>99</v>
@@ -3799,10 +3808,13 @@
       <c r="K50" s="1" t="inlineStr">
         <is>
           <t>"building = hotel", 2
-"tourism = guest_house", 7
-"building = house", 2
+"tourism = guest_house", 8
+"building = house", 3
 "place = locality", 7
-"place = hamlet", 2</t>
+"place = hamlet", 2
+"building = yes", 2
+"ref:bygningsnr = 165884418", 2
+"ref:bygningsnr = 165877926", 2</t>
         </is>
       </c>
       <c r="L50" s="17" t="inlineStr">
@@ -3838,7 +3850,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>1036</v>
+        <v>1039</v>
       </c>
       <c r="G51" s="12" t="n">
         <v>784</v>
@@ -3865,12 +3877,12 @@
 "network = Den Norske Turistforening", 10
 "shelter_type = basic_hut", 3
 "tourism = wilderness_hut", 11
-"building = cabin", 10
+"building = cabin", 11
 "capacity = 11", 2
 "dnt:classification = ubetjent", 11
 "dnt:lock = yes", 15
-"tourism = alpine_hut", 3
-"tourism = chalet", 48
+"tourism = alpine_hut", 4
+"tourism = chalet", 52
 "amenity = cafe", 11
 "capacity = 24", 2
 "dnt:classification = servering", 5
@@ -3895,6 +3907,7 @@
 "ski = yes", 2
 "ref:bygningsnr = 165795091", 2
 "ref:bygningsnr = 165767705", 2
+"ref:bygningsnr = 165906551", 2
 "amenity = restaurant", 2</t>
         </is>
       </c>
@@ -3936,7 +3949,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G52" s="12" t="n">
         <v>152</v>
@@ -4062,7 +4075,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G54" s="12" t="n">
         <v>29</v>
@@ -4195,7 +4208,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="G57" s="12" t="n">
         <v>463</v>
@@ -4217,7 +4230,7 @@
       </c>
       <c r="K57" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 9</t>
+          <t>"place = locality", 11</t>
         </is>
       </c>
       <c r="M57" s="12" t="inlineStr">
@@ -4253,7 +4266,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1072</v>
+        <v>1100</v>
       </c>
       <c r="G58" s="12" t="n">
         <v>1042</v>
@@ -4275,7 +4288,7 @@
       </c>
       <c r="K58" s="1" t="inlineStr">
         <is>
-          <t>"natural = strait", 66
+          <t>"natural = strait", 69
 "place = locality", 4</t>
         </is>
       </c>
@@ -4312,7 +4325,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>7253</v>
+        <v>7389</v>
       </c>
       <c r="G59" s="12" t="n">
         <v>7211</v>
@@ -4334,7 +4347,7 @@
       </c>
       <c r="K59" s="1" t="inlineStr">
         <is>
-          <t>"natural = bay", 252</t>
+          <t>"natural = bay", 283</t>
         </is>
       </c>
       <c r="L59" s="17" t="inlineStr">
@@ -4370,7 +4383,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>1313</v>
+        <v>1371</v>
       </c>
       <c r="G60" s="12" t="n">
         <v>1296</v>
@@ -4393,7 +4406,7 @@
       <c r="K60" s="1" t="inlineStr">
         <is>
           <t>"place = island", 95
-"place = islet", 4</t>
+"place = islet", 6</t>
         </is>
       </c>
       <c r="L60" s="17" t="inlineStr">
@@ -4429,7 +4442,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>4201</v>
+        <v>4177</v>
       </c>
       <c r="G61" s="12" t="n">
         <v>4298</v>
@@ -4451,8 +4464,8 @@
       </c>
       <c r="K61" s="1" t="inlineStr">
         <is>
-          <t>"natural = wood", 25
-"place = islet", 150</t>
+          <t>"natural = wood", 26
+"place = islet", 157</t>
         </is>
       </c>
       <c r="L61" s="17" t="inlineStr">
@@ -4488,7 +4501,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="G62" s="12" t="n">
         <v>255</v>
@@ -4510,7 +4523,7 @@
       </c>
       <c r="K62" s="1" t="inlineStr">
         <is>
-          <t>"natural = cape", 30</t>
+          <t>"natural = cape", 41</t>
         </is>
       </c>
       <c r="L62" s="2" t="inlineStr">
@@ -4546,7 +4559,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>9527</v>
+        <v>9684</v>
       </c>
       <c r="G63" s="12" t="n">
         <v>9498</v>
@@ -4568,7 +4581,7 @@
       </c>
       <c r="K63" s="1" t="inlineStr">
         <is>
-          <t>"natural = cape", 327</t>
+          <t>"natural = cape", 382</t>
         </is>
       </c>
       <c r="L63" s="17" t="inlineStr">
@@ -4604,7 +4617,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G64" s="12" t="n">
         <v>390</v>
@@ -4663,7 +4676,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>990</v>
+        <v>985</v>
       </c>
       <c r="G65" s="12" t="n">
         <v>923</v>
@@ -4724,7 +4737,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G66" s="12" t="n">
         <v>73</v>
@@ -4782,7 +4795,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>416</v>
+        <v>435</v>
       </c>
       <c r="G67" s="12" t="n">
         <v>399</v>
@@ -4804,7 +4817,8 @@
       </c>
       <c r="K67" s="1" t="inlineStr">
         <is>
-          <t>"place = islet", 4</t>
+          <t>"place = islet", 4
+"natural = shoal", 2</t>
         </is>
       </c>
       <c r="L67" s="17" t="inlineStr">
@@ -4901,7 +4915,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G69" s="12" t="n">
         <v>199</v>
@@ -5019,7 +5033,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>9497</v>
+        <v>9553</v>
       </c>
       <c r="G71" s="12" t="n">
         <v>10146</v>
@@ -5081,7 +5095,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>43141</v>
+        <v>43255</v>
       </c>
       <c r="G72" s="12" t="n">
         <v>44547</v>
@@ -5103,10 +5117,10 @@
       </c>
       <c r="K72" s="1" t="inlineStr">
         <is>
-          <t>"waterway = stream", 464
+          <t>"waterway = stream", 465
 "layer = -1", 72
 "tunnel = culvert", 20
-"waterway = river", 57
+"waterway = river", 56
 "width = 2", 80
 "width = 3", 24
 "place = locality", 76</t>
@@ -5196,7 +5210,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>3431</v>
+        <v>3421</v>
       </c>
       <c r="G74" s="12" t="n">
         <v>3394</v>
@@ -5218,8 +5232,8 @@
       </c>
       <c r="K74" s="1" t="inlineStr">
         <is>
-          <t>"natural = waterfall", 23
-"waterway = waterfall", 8
+          <t>"natural = waterfall", 25
+"waterway = waterfall", 9
 "place = locality", 9
 "water = waterfall", 3</t>
         </is>
@@ -5257,7 +5271,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G75" s="12" t="n">
         <v>461</v>
@@ -5321,7 +5335,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>1019</v>
+        <v>1035</v>
       </c>
       <c r="G76" s="12" t="n">
         <v>1004</v>
@@ -5379,7 +5393,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>2565</v>
+        <v>2629</v>
       </c>
       <c r="G77" s="12" t="n">
         <v>2461</v>
@@ -5405,7 +5419,7 @@
 "type = multipolygon", 3
 "water = pool", 5
 "water = pond", 3
-"place = locality", 17</t>
+"place = locality", 18</t>
         </is>
       </c>
       <c r="L77" s="2" t="n"/>
@@ -5447,7 +5461,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>1770</v>
+        <v>1856</v>
       </c>
       <c r="G78" s="12" t="n">
         <v>1780</v>
@@ -5508,7 +5522,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G79" s="12" t="n">
         <v>15</v>
@@ -5530,7 +5544,7 @@
       </c>
       <c r="K79" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 3</t>
+          <t>"place = locality", 4</t>
         </is>
       </c>
       <c r="M79" s="17" t="inlineStr">
@@ -5566,7 +5580,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>676</v>
+        <v>665</v>
       </c>
       <c r="G80" s="12" t="n">
         <v>654</v>
@@ -5588,7 +5602,7 @@
       </c>
       <c r="K80" s="1" t="inlineStr">
         <is>
-          <t>"natural = cape", 17</t>
+          <t>"natural = cape", 23</t>
         </is>
       </c>
       <c r="L80" s="17" t="inlineStr">
@@ -5625,7 +5639,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G81" s="12" t="n">
         <v>126</v>
@@ -5735,7 +5749,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="G83" s="12" t="n">
         <v>470</v>
@@ -5757,12 +5771,12 @@
       </c>
       <c r="K83" s="1" t="inlineStr">
         <is>
-          <t>"natural = water", 19
-"type = multipolygon", 19
-"water = lake", 15
-"ele:min = 431", 4
-"intermittent = no", 4
-"salt = no", 4</t>
+          <t>"natural = water", 18
+"type = multipolygon", 18
+"water = lake", 14
+"ele:min = 431", 3
+"intermittent = no", 3
+"salt = no", 3</t>
         </is>
       </c>
       <c r="L83" s="17" t="inlineStr">
@@ -5798,7 +5812,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>13032</v>
+        <v>13111</v>
       </c>
       <c r="G84" s="12" t="n">
         <v>14069</v>
@@ -5820,10 +5834,9 @@
       </c>
       <c r="K84" s="1" t="inlineStr">
         <is>
-          <t>"natural = water", 437
-"type = multipolygon", 333
-"water = lake", 288
-"water = reservoir", 17</t>
+          <t>"natural = water", 443
+"type = multipolygon", 338
+"water = lake", 294</t>
         </is>
       </c>
       <c r="L84" s="17" t="inlineStr">
@@ -5859,7 +5872,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>56978</v>
+        <v>58099</v>
       </c>
       <c r="G85" s="12" t="n">
         <v>62457</v>
@@ -5881,9 +5894,9 @@
       </c>
       <c r="K85" s="1" t="inlineStr">
         <is>
-          <t>"natural = water", 3084
-"type = multipolygon", 1488
-"water = lake", 900</t>
+          <t>"natural = water", 3124
+"type = multipolygon", 1515
+"water = lake", 940</t>
         </is>
       </c>
       <c r="L85" s="17" t="inlineStr">
@@ -5919,7 +5932,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="G86" s="12" t="n">
         <v>1286</v>
@@ -5941,10 +5954,10 @@
       </c>
       <c r="K86" s="1" t="inlineStr">
         <is>
-          <t>"natural = water", 102
-"water = pond", 104
+          <t>"natural = water", 103
+"water = pond", 105
 "place = locality", 7
-"type = multipolygon", 10</t>
+"type = multipolygon", 11</t>
         </is>
       </c>
       <c r="L86" s="17" t="inlineStr">
@@ -5980,7 +5993,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>867</v>
+        <v>837</v>
       </c>
       <c r="G87" s="12" t="n">
         <v>884</v>
@@ -6040,7 +6053,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G88" s="12" t="n">
         <v>129</v>
@@ -6101,7 +6114,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="G89" s="12" t="n">
         <v>166</v>
@@ -6163,7 +6176,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>2496</v>
+        <v>2444</v>
       </c>
       <c r="G90" s="12" t="n">
         <v>687</v>
@@ -6257,7 +6270,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="G92" s="12" t="n">
         <v>506</v>
@@ -6327,7 +6340,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="G93" s="12" t="n">
         <v>215</v>
@@ -6479,7 +6492,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I96" s="2" t="inlineStr">
         <is>
@@ -6521,7 +6534,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G97" s="12" t="n">
         <v>174</v>
@@ -6930,7 +6943,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G105" s="12" t="n">
         <v>120</v>
@@ -6990,7 +7003,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G106" s="12" t="n">
         <v>22</v>
@@ -7084,7 +7097,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G108" s="12" t="n">
         <v>98</v>
@@ -7138,7 +7151,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>2195</v>
+        <v>2151</v>
       </c>
       <c r="G109" s="12" t="n">
         <v>2333</v>
@@ -7209,7 +7222,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G110" s="12" t="n">
         <v>202</v>
@@ -7273,7 +7286,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>506</v>
+        <v>533</v>
       </c>
       <c r="G111" s="12" t="n">
         <v>490</v>
@@ -7633,7 +7646,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G119" s="12" t="n">
         <v>118</v>
@@ -7694,7 +7707,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>198</v>
+        <v>1400</v>
       </c>
       <c r="G120" s="12" t="n">
         <v>1216</v>
@@ -7716,19 +7729,33 @@
       </c>
       <c r="K120" s="1" t="inlineStr">
         <is>
-          <t>"layer = -1", 7
-"surface = paved", 2
-"tunnel = yes", 7
-"electrified = contact_line", 3
-"frequency = 16.67", 3
-"gauge = 1435", 3
-"maxspeed:hgv = 80", 2
-"maxspeed:plus = 85", 2
-"maxspeed:tilting = 100", 2
-"passenger_lines = 1", 3
-"railway = rail", 3
-"usage = main", 3
-"voltage = 15000", 3
+          <t>"layer = -1", 15
+"surface = paved", 3
+"tunnel = yes", 19
+"bicycle = no", 3
+"foot = no", 3
+"highway = primary", 8
+"lit = yes", 7
+"surface = asphalt", 5
+"bicycle = yes", 2
+"foot = yes", 3
+"maxheight = 4.2", 2
+"highway = trunk", 2
+"int_ref = E 39", 2
+"maxheight = 4.5", 2
+"electrified = contact_line", 6
+"frequency = 16.67", 6
+"gauge = 1435", 6
+"maxspeed:hgv = 80", 4
+"maxspeed:plus = 85", 4
+"maxspeed:tilting = 100", 4
+"passenger_lines = 1", 6
+"railway = rail", 6
+"usage = main", 6
+"voltage = 15000", 6
+"maxspeed:hgv = 90", 2
+"maxspeed:plus = 100", 2
+"maxspeed:tilting = 115", 2
 "is_in:continent = Europe", 2
 "is_in:country = Norway", 2
 "is_in:country_code = NO", 2
@@ -7762,7 +7789,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>8535</v>
+        <v>9913</v>
       </c>
       <c r="I121" s="2" t="inlineStr">
         <is>
@@ -7772,29 +7799,36 @@
       <c r="J121" s="14" t="n"/>
       <c r="K121" s="1" t="inlineStr">
         <is>
-          <t>"layer = -1", 3
+          <t>"bridge = yes", 61
+"layer = 1", 65
+"surface = asphalt", 13
+"man_made = bridge", 30
+"layer = -1", 3
 "man_made = tunnel", 3
-"bridge = yes", 48
 "cycleway:both = no", 4
-"highway = primary", 18
-"layer = 1", 50
-"surface = asphalt", 12
+"highway = primary", 19
 "lanes = 2", 6
-"maxweight:signed = no", 3
-"highway = secondary", 11
+"maxweight:signed = no", 4
+"highway = secondary", 14
 "highway = service", 2
-"highway = trunk", 2
-"surface = paved", 2
-"man_made = bridge", 26
+"highway = trunk", 4
+"surface = paved", 3
 "tunnel = culvert", 8
-"waterway = stream", 9
+"waterway = stream", 10
 "VANNBR = 2", 2
 "bridge:description = Dragbrua", 2
 "surface = gravel", 2
 "bridge:description = Grymyr", 2
 "place = suburb", 2
+"old_ref = 459", 2
+"highway = tertiary", 2
+"int_ref = E 39", 2
+"lit = yes", 2
+"highway = track", 4
+"nvdb:id = 339480834", 2
+"old_ref = 202", 2
+"old_ref = 408", 2
 "highway = residential", 2
-"highway = track", 2
 "historic = bridge", 2
 "place = locality", 4
 "old_ref = 158", 2
@@ -8302,7 +8336,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="G132" s="12" t="n">
         <v>341</v>
@@ -8371,7 +8405,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="G133" s="12" t="n">
         <v>407</v>
@@ -8394,8 +8428,9 @@
       <c r="K133" s="1" t="inlineStr">
         <is>
           <t>"place = isolated_dwelling", 2
-"man_made = quay", 14
-"place = locality", 15</t>
+"man_made = quay", 19
+"place = locality", 22
+"natural = coastline", 2</t>
         </is>
       </c>
       <c r="L133" s="17" t="inlineStr">
@@ -8441,7 +8476,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="G134" s="12" t="n">
         <v>160</v>
@@ -8606,7 +8641,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="G137" s="12" t="n">
         <v>64</v>
@@ -8716,7 +8751,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="G139" s="12" t="n">
         <v>65</v>
@@ -8738,9 +8773,10 @@
       </c>
       <c r="K139" s="1" t="inlineStr">
         <is>
-          <t>"natural = beach", 2
-"surface = sand", 2
-"leisure = marina", 2</t>
+          <t>"place = locality", 2
+"leisure = marina", 3
+"natural = beach", 2
+"surface = sand", 2</t>
         </is>
       </c>
       <c r="L139" s="17" t="inlineStr">
@@ -8781,7 +8817,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="G140" s="12" t="n">
         <v>188</v>
@@ -8844,7 +8880,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="G141" s="12" t="n">
         <v>400</v>
@@ -8866,8 +8902,8 @@
       </c>
       <c r="K141" s="1" t="inlineStr">
         <is>
-          <t>"mooring = yes", 5
-"place = locality", 93
+          <t>"mooring = yes", 6
+"place = locality", 94
 "historic = yes", 92</t>
         </is>
       </c>
@@ -8980,7 +9016,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>6927</v>
+        <v>104074</v>
       </c>
       <c r="G143" s="12" t="n">
         <v>24621</v>
@@ -9002,8 +9038,8 @@
       </c>
       <c r="K143" s="1" t="inlineStr">
         <is>
-          <t>"natural = coastline", 2
-"place = islet", 2</t>
+          <t>"place = islet", 3
+"natural = coastline", 2</t>
         </is>
       </c>
       <c r="O143" s="17">
@@ -9039,7 +9075,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>747</v>
+        <v>692</v>
       </c>
       <c r="G144" s="12" t="n">
         <v>729</v>
@@ -9061,11 +9097,11 @@
       </c>
       <c r="K144" s="1" t="inlineStr">
         <is>
-          <t>"highway = track", 13
+          <t>"highway = track", 14
 "tracktype = grade3", 2
-"tracktype = grade4", 2
+"tracktype = grade4", 3
 "place = locality", 6
-"highway = path", 2</t>
+"highway = path", 3</t>
         </is>
       </c>
       <c r="L144" s="9" t="inlineStr">
@@ -9106,7 +9142,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>4382</v>
+        <v>4452</v>
       </c>
       <c r="G145" s="12" t="n">
         <v>4064</v>
@@ -9132,7 +9168,7 @@
 "sac_scale = hiking", 6
 "mtb:scale = 1", 2
 "trail_visibility = excellent", 3
-"place = locality", 17</t>
+"place = locality", 18</t>
         </is>
       </c>
       <c r="L145" s="9" t="inlineStr">
@@ -9168,7 +9204,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>741</v>
+        <v>760</v>
       </c>
       <c r="G146" s="12" t="n">
         <v>673</v>
@@ -9232,7 +9268,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G147" s="12" t="n">
         <v>70</v>
@@ -9398,7 +9434,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>885</v>
+        <v>916</v>
       </c>
       <c r="G150" s="12" t="n">
         <v>788</v>
@@ -9467,7 +9503,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G151" s="12" t="n">
         <v>261</v>
@@ -9525,7 +9561,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>1066</v>
+        <v>1125</v>
       </c>
       <c r="G152" s="12" t="n">
         <v>792</v>
@@ -9832,7 +9868,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>1716</v>
+        <v>1704</v>
       </c>
       <c r="G159" s="12" t="n">
         <v>1629</v>
@@ -9854,49 +9890,40 @@
       </c>
       <c r="K159" s="1" t="inlineStr">
         <is>
-          <t>"amenity = place_of_worship", 98
-"denomination = lutheran", 97
+          <t>"amenity = place_of_worship", 101
+"denomination = lutheran", 100
 "diocese = Stavanger", 15
-"religion = christian", 98
+"religion = christian", 101
 "toilets = no", 9
 "toilets:wheelchair = no", 6
-"wheelchair = limited", 3
-"building = church", 93
-"capacity = 700", 3
+"building = church", 96
 "deanery = Ytre Stavanger", 6
 "note = Soknekirke/arbeidskirke", 12
 "toilets = yes", 45
 "deanery = Stavanger Domprosti", 7
-"note = Soknekirke", 41
+"note = Soknekirke", 43
 "capacity = 300", 5
 "toilets:wheelchair = yes", 10
 "wheelchair = yes", 12
 "note = Prostikirke", 4
-"capacity = 430", 3
 "capacity = 500", 10
 "capacity = 450", 6
-"capacity = 650", 3
-"capacity = 400", 3
 "deanery = Bodø Domprosti", 6
 "diocese = Sør-Hålogaland", 6
-"heritage = yes", 54
-"parish = Gildeskål", 3
+"heritage = yes", 57
 "capacity = 250", 7
 "diocese = Tunsberg", 13
 "deanery = Kongsberg", 7
 "hearing_aids = yes", 15
-"parish = Kongsberg og Jondalen", 3
-"capacity = 150", 3
 "architect = J.W.Nordan", 4
-"capacity = 170", 3
 "capacity = 200", 10
 "deanery = Lier", 4
 "architect = J.H.Nissen", 4
 "deanery = Aust-Nedenes", 20
-"diocese = Agder og Telemark", 57
-"deanery = Mandal", 3
+"diocese = Agder og Telemark", 60
+"deanery = Mandal", 6
+"parish = Mandal", 4
 "deanery = Lister", 4
-"parish = Farsund", 3
 "capacity = 350", 8
 "parish = Holt", 4
 "deanery = Vest-Nedenes", 6
@@ -9947,7 +9974,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>785</v>
+        <v>802</v>
       </c>
       <c r="G160" s="12" t="n">
         <v>653</v>
@@ -9972,7 +9999,10 @@
           <t>"amenity = community_centre", 15
 "place = isolated_dwelling", 4
 "place = farm", 2
-"building = civic", 4</t>
+"building = civic", 5
+"place = locality", 2
+"heritage = yes", 2
+"ref:bygningsnr = 168600461", 2</t>
         </is>
       </c>
       <c r="L160" s="17" t="inlineStr">
@@ -10008,7 +10038,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G161" s="12" t="n">
         <v>127</v>
@@ -10079,7 +10109,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G162" s="12" t="n">
         <v>70</v>
@@ -10142,7 +10172,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G163" s="12" t="n">
         <v>98</v>
@@ -10293,7 +10323,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G166" s="12" t="n">
         <v>193</v>
@@ -10319,7 +10349,7 @@
 "tourism = museum", 2
 "type = multipolygon", 2
 "place = locality", 3
-"historic = memorial", 3</t>
+"historic = memorial", 4</t>
         </is>
       </c>
       <c r="L166" s="17" t="inlineStr">
@@ -10355,7 +10385,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G167" s="12" t="n">
         <v>97</v>
@@ -10409,7 +10439,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>5029</v>
+        <v>5335</v>
       </c>
       <c r="G168" s="12" t="n">
         <v>3733</v>
@@ -10431,13 +10461,13 @@
       </c>
       <c r="K168" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 242
-"building = farm_auxiliary", 25
+          <t>"place = locality", 267
+"building = farm_auxiliary", 26
 "man_made = mineshaft", 18
 "resource = silver", 21
 "historic = mine", 40
-"place = isolated_dwelling", 13
-"historic = shieling", 10</t>
+"place = isolated_dwelling", 35
+"historic = shieling", 11</t>
         </is>
       </c>
       <c r="M168" s="12" t="inlineStr">
@@ -10473,7 +10503,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>518</v>
+        <v>552</v>
       </c>
       <c r="G169" s="12" t="n">
         <v>444</v>
@@ -10569,7 +10599,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>5984</v>
+        <v>6008</v>
       </c>
       <c r="G171" s="12" t="n">
         <v>5340</v>
@@ -10591,8 +10621,8 @@
       </c>
       <c r="K171" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 117
-"place = farm", 21</t>
+          <t>"place = locality", 120
+"place = farm", 23</t>
         </is>
       </c>
       <c r="L171" s="2" t="n"/>
@@ -10634,7 +10664,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>3003</v>
+        <v>3093</v>
       </c>
       <c r="G172" s="12" t="n">
         <v>2408</v>
@@ -10658,7 +10688,7 @@
         <is>
           <t>"landuse = meadow", 24
 "type = multipolygon", 4
-"place = locality", 26
+"place = locality", 31
 "natural = wetland", 2
 "wetland = bog", 2</t>
         </is>
@@ -10696,7 +10726,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>7661</v>
+        <v>8251</v>
       </c>
       <c r="G173" s="12" t="n">
         <v>4914</v>
@@ -10718,11 +10748,9 @@
       </c>
       <c r="K173" s="1" t="inlineStr">
         <is>
-          <t>"landuse = farmland", 40
-"type = multipolygon", 19
-"place = farm", 7
-"place = isolated_dwelling", 7
-"place = locality", 155</t>
+          <t>"landuse = farmland", 48
+"type = multipolygon", 22
+"place = locality", 209</t>
         </is>
       </c>
       <c r="M173" s="12" t="inlineStr">
@@ -10758,7 +10786,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>498</v>
+        <v>526</v>
       </c>
       <c r="G174" s="12" t="n">
         <v>314</v>
@@ -10780,7 +10808,7 @@
       </c>
       <c r="K174" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 12</t>
+          <t>"place = locality", 14</t>
         </is>
       </c>
       <c r="M174" s="17" t="inlineStr">
@@ -10821,7 +10849,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>3630</v>
+        <v>3740</v>
       </c>
       <c r="G175" s="12" t="n">
         <v>3166</v>
@@ -10843,11 +10871,11 @@
       </c>
       <c r="K175" s="1" t="inlineStr">
         <is>
-          <t>"historic = shieling", 138
+          <t>"historic = shieling", 143
 "landuse = meadow", 26
-"place = locality", 165
+"place = locality", 172
 "place = isolated_dwelling", 6
-"place = farm", 11</t>
+"place = farm", 14</t>
         </is>
       </c>
       <c r="L175" s="2" t="inlineStr">
@@ -10888,7 +10916,7 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="G176" s="12" t="n">
         <v>264</v>
@@ -10952,7 +10980,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>485</v>
+        <v>416</v>
       </c>
       <c r="G177" s="12" t="n">
         <v>491</v>
@@ -11012,7 +11040,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G178" s="12" t="n">
         <v>179</v>
@@ -11103,7 +11131,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>3280</v>
+        <v>3268</v>
       </c>
       <c r="G180" s="12" t="n">
         <v>2950</v>
@@ -11125,7 +11153,7 @@
       </c>
       <c r="K180" s="1" t="inlineStr">
         <is>
-          <t>"natural = stone", 44
+          <t>"natural = stone", 53
 "place = locality", 4
 "natural = rock", 2</t>
         </is>
@@ -11164,7 +11192,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>2482</v>
+        <v>2414</v>
       </c>
       <c r="G181" s="12" t="n">
         <v>2354</v>
@@ -11186,7 +11214,7 @@
       </c>
       <c r="K181" s="1" t="inlineStr">
         <is>
-          <t>"natural = scree", 68
+          <t>"natural = scree", 81
 "place = locality", 20</t>
         </is>
       </c>
@@ -11274,7 +11302,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G183" s="12" t="n">
         <v>121</v>
@@ -11294,7 +11322,11 @@
           <t>Sand-/grusområde over vannkontur/kystkontur; morenemateriale</t>
         </is>
       </c>
-      <c r="K183" s="1" t="inlineStr"/>
+      <c r="K183" s="1" t="inlineStr">
+        <is>
+          <t>"place = locality", 2</t>
+        </is>
+      </c>
       <c r="L183" s="17" t="inlineStr">
         <is>
           <t>natural=beach; surface=sand</t>
@@ -11458,7 +11490,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="G187" s="12" t="n">
         <v>273</v>
@@ -11519,7 +11551,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G188" s="12" t="n">
         <v>127</v>
@@ -11629,7 +11661,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>7449</v>
+        <v>7826</v>
       </c>
       <c r="G190" s="12" t="n">
         <v>7616</v>
@@ -11651,12 +11683,11 @@
       </c>
       <c r="K190" s="1" t="inlineStr">
         <is>
-          <t>"leaf_type = needleleaved", 3
-"natural = wood", 20
+          <t>"natural = wood", 20
 "type = multipolygon", 6
-"place = locality", 99
+"place = locality", 101
 "place = isolated_dwelling", 5
-"place = farm", 8</t>
+"place = farm", 11</t>
         </is>
       </c>
       <c r="M190" s="12" t="inlineStr">
@@ -11692,7 +11723,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="G191" s="12" t="n">
         <v>6</v>
@@ -11750,7 +11781,7 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>49387</v>
+        <v>50297</v>
       </c>
       <c r="G192" s="12" t="n">
         <v>50738</v>
@@ -11772,8 +11803,8 @@
       </c>
       <c r="K192" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 440
-"natural = wetland", 738
+          <t>"place = locality", 665
+"natural = wetland", 737
 "wetland = bog", 258
 "type = multipolygon", 97</t>
         </is>
@@ -11999,7 +12030,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G197" s="12" t="n">
         <v>12</v>
@@ -12481,7 +12512,7 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="G207" s="12" t="n">
         <v>233</v>
@@ -12591,7 +12622,7 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>818</v>
+        <v>948</v>
       </c>
       <c r="G209" s="12" t="n">
         <v>302</v>
@@ -12718,7 +12749,7 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G211" s="12" t="n">
         <v>72</v>
@@ -12861,7 +12892,7 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>1953</v>
+        <v>1903</v>
       </c>
       <c r="G214" s="12" t="n">
         <v>1901</v>
@@ -12883,9 +12914,9 @@
       </c>
       <c r="K214" s="1" t="inlineStr">
         <is>
-          <t>"bay = fjord", 126
-"natural = bay", 128
-"type = multipolygon", 14</t>
+          <t>"bay = fjord", 143
+"natural = bay", 145
+"type = multipolygon", 15</t>
         </is>
       </c>
       <c r="L214" s="17" t="inlineStr">
@@ -13029,7 +13060,7 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G217" s="12" t="n">
         <v>119</v>
@@ -13049,7 +13080,11 @@
           <t>Del av sjøen, vanligvis innaskjærs eller i kystnære farvann. Eks. Folda, Hustadvika</t>
         </is>
       </c>
-      <c r="K217" s="1" t="inlineStr"/>
+      <c r="K217" s="1" t="inlineStr">
+        <is>
+          <t>"place = locality", 2</t>
+        </is>
+      </c>
       <c r="L217" s="17" t="inlineStr">
         <is>
           <t>natural=bay</t>
@@ -13088,9 +13123,6 @@
           <t>fiskeplassISjø</t>
         </is>
       </c>
-      <c r="F218" t="n">
-        <v>53</v>
-      </c>
       <c r="G218" s="12" t="n">
         <v>46</v>
       </c>
@@ -13109,7 +13141,7 @@
           <t>Fiskested, fiskemed</t>
         </is>
       </c>
-      <c r="K218" s="1" t="inlineStr"/>
+      <c r="K218" s="17" t="n"/>
       <c r="M218" s="12" t="n"/>
       <c r="O218" s="17">
         <f>CONCATENATE(Tabell1[[#This Row],[OSM tag]],";",Tabell1[[#This Row],[tillegg]],";",Tabell1[[#This Row],[fixme]])</f>
@@ -13190,7 +13222,7 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>13440</v>
+        <v>13248</v>
       </c>
       <c r="G220" s="12" t="n">
         <v>13989</v>
@@ -13213,10 +13245,10 @@
       <c r="K220" s="1" t="inlineStr">
         <is>
           <t>"natural = rock", 345
-"seamark:type = rock", 91
-"place = islet", 457
-"natural = coastline", 379
-"natural = shoal", 42</t>
+"seamark:type = rock", 126
+"place = islet", 586
+"natural = coastline", 473
+"natural = shoal", 78</t>
         </is>
       </c>
       <c r="L220" s="17" t="inlineStr">
@@ -13257,7 +13289,7 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>1195</v>
+        <v>1230</v>
       </c>
       <c r="G221" s="12" t="n">
         <v>1206</v>
@@ -13280,8 +13312,8 @@
       <c r="K221" s="1" t="inlineStr">
         <is>
           <t>"natural = rock", 2
-"place = locality", 37
-"seamark:type = rock", 37</t>
+"place = locality", 65
+"seamark:type = rock", 65</t>
         </is>
       </c>
       <c r="L221" s="17" t="inlineStr">
@@ -13327,7 +13359,7 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>13195</v>
+        <v>12733</v>
       </c>
       <c r="G222" s="12" t="n">
         <v>13694</v>
@@ -13349,8 +13381,8 @@
       </c>
       <c r="K222" s="1" t="inlineStr">
         <is>
-          <t>"natural = shoal", 336
-"place = locality", 129</t>
+          <t>"natural = shoal", 355
+"place = locality", 148</t>
         </is>
       </c>
       <c r="L222" s="17" t="inlineStr">
@@ -13443,7 +13475,7 @@
         </is>
       </c>
       <c r="F224" t="n">
-        <v>4572</v>
+        <v>4258</v>
       </c>
       <c r="G224" s="12" t="n">
         <v>4494</v>
@@ -13465,7 +13497,7 @@
       </c>
       <c r="K224" s="1" t="inlineStr">
         <is>
-          <t>"natural = strait", 339</t>
+          <t>"natural = strait", 395</t>
         </is>
       </c>
       <c r="L224" s="17" t="inlineStr">
@@ -13501,7 +13533,7 @@
         </is>
       </c>
       <c r="F225" t="n">
-        <v>25792</v>
+        <v>25086</v>
       </c>
       <c r="G225" s="12" t="n">
         <v>26737</v>
@@ -13523,7 +13555,7 @@
       </c>
       <c r="K225" s="1" t="inlineStr">
         <is>
-          <t>"natural = bay", 1419</t>
+          <t>"natural = bay", 1686</t>
         </is>
       </c>
       <c r="L225" s="17" t="inlineStr">
@@ -13560,7 +13592,7 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>3809</v>
+        <v>3757</v>
       </c>
       <c r="G226" s="12" t="n">
         <v>4179</v>
@@ -13582,10 +13614,10 @@
       </c>
       <c r="K226" s="1" t="inlineStr">
         <is>
-          <t>"place = island", 121
-"natural = coastline", 117
-"place = islet", 107
-"type = multipolygon", 93
+          <t>"place = island", 123
+"natural = coastline", 131
+"place = islet", 131
+"type = multipolygon", 105
 "natural = wood", 8</t>
         </is>
       </c>
@@ -13622,7 +13654,7 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>19062</v>
+        <v>18301</v>
       </c>
       <c r="G227" s="12" t="n">
         <v>20058</v>
@@ -13644,9 +13676,9 @@
       </c>
       <c r="K227" s="1" t="inlineStr">
         <is>
-          <t>"place = islet", 1175
-"natural = coastline", 1054
-"type = multipolygon", 86</t>
+          <t>"place = islet", 1338
+"natural = coastline", 1193
+"type = multipolygon", 109</t>
         </is>
       </c>
       <c r="L227" s="17" t="inlineStr">
@@ -13682,7 +13714,7 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>505</v>
+        <v>524</v>
       </c>
       <c r="G228" s="12" t="n">
         <v>495</v>
@@ -13705,7 +13737,7 @@
       <c r="K228" s="1" t="inlineStr">
         <is>
           <t>"place = locality", 9
-"natural = cape", 30</t>
+"natural = cape", 50</t>
         </is>
       </c>
       <c r="L228" s="17" t="inlineStr">
@@ -13741,7 +13773,7 @@
         </is>
       </c>
       <c r="F229" t="n">
-        <v>22726</v>
+        <v>21874</v>
       </c>
       <c r="G229" s="12" t="n">
         <v>24024</v>
@@ -13763,7 +13795,7 @@
       </c>
       <c r="K229" s="1" t="inlineStr">
         <is>
-          <t>"natural = cape", 838
+          <t>"natural = cape", 1012
 "place = locality", 54</t>
         </is>
       </c>
@@ -13801,7 +13833,7 @@
         </is>
       </c>
       <c r="F230" t="n">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="G230" s="12" t="n">
         <v>240</v>
@@ -13823,7 +13855,7 @@
       </c>
       <c r="K230" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 2</t>
+          <t>"place = locality", 3</t>
         </is>
       </c>
       <c r="M230" s="17" t="inlineStr">
@@ -13859,7 +13891,7 @@
         </is>
       </c>
       <c r="F231" t="n">
-        <v>2307</v>
+        <v>2323</v>
       </c>
       <c r="G231" s="12" t="n">
         <v>2328</v>
@@ -13881,12 +13913,12 @@
       </c>
       <c r="K231" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 34
-"natural = beach", 47
-"type = multipolygon", 8
+          <t>"place = locality", 40
+"natural = beach", 52
+"type = multipolygon", 9
 "place = isolated_dwelling", 2
-"layer = 2", 3
-"surface = sand", 9
+"layer = 2", 7
+"surface = sand", 13
 "place = hamlet", 2</t>
         </is>
       </c>
@@ -13924,7 +13956,7 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>1437</v>
+        <v>1211</v>
       </c>
       <c r="G232" s="12" t="n">
         <v>1405</v>
@@ -13946,7 +13978,7 @@
       </c>
       <c r="K232" s="1" t="inlineStr">
         <is>
-          <t>"natural = bay", 19</t>
+          <t>"natural = bay", 22</t>
         </is>
       </c>
       <c r="L232" s="17" t="inlineStr">
@@ -13983,7 +14015,7 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G233" s="12" t="n">
         <v>351</v>
@@ -14007,8 +14039,10 @@
         <is>
           <t>"place = archipelago", 2
 "place = island", 6
-"natural = coastline", 13
-"place = islet", 11</t>
+"natural = coastline", 20
+"place = islet", 20
+"natural = cape", 2
+"type = multipolygon", 3</t>
         </is>
       </c>
       <c r="L233" s="17" t="inlineStr">
@@ -14044,7 +14078,7 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="G234" s="12" t="n">
         <v>318</v>
@@ -14066,8 +14100,8 @@
       </c>
       <c r="K234" s="1" t="inlineStr">
         <is>
-          <t>"natural = coastline", 14
-"place = islet", 15</t>
+          <t>"natural = coastline", 18
+"place = islet", 19</t>
         </is>
       </c>
       <c r="L234" s="17" t="inlineStr">
@@ -14104,7 +14138,7 @@
         </is>
       </c>
       <c r="F235" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G235" s="12" t="n">
         <v>109</v>
@@ -14201,7 +14235,7 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G237" s="12" t="n">
         <v>78</v>
@@ -14221,7 +14255,11 @@
           <t>Skrånende sjøbunn; skråning</t>
         </is>
       </c>
-      <c r="K237" s="1" t="inlineStr"/>
+      <c r="K237" s="1" t="inlineStr">
+        <is>
+          <t>"place = locality", 2</t>
+        </is>
+      </c>
       <c r="M237" s="11" t="n"/>
       <c r="O237" s="17">
         <f>CONCATENATE(Tabell1[[#This Row],[OSM tag]],";",Tabell1[[#This Row],[tillegg]],";",Tabell1[[#This Row],[fixme]])</f>
@@ -14933,7 +14971,7 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>7855</v>
+        <v>7562</v>
       </c>
       <c r="G258" s="12" t="n">
         <v>7739</v>
@@ -14955,7 +14993,7 @@
       </c>
       <c r="K258" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 193</t>
+          <t>"place = locality", 209</t>
         </is>
       </c>
       <c r="L258" s="2" t="n"/>
@@ -14992,7 +15030,7 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>4124</v>
+        <v>4225</v>
       </c>
       <c r="G259" s="12" t="n">
         <v>4173</v>
@@ -15050,7 +15088,7 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>15086</v>
+        <v>14743</v>
       </c>
       <c r="G260" s="12" t="n">
         <v>15244</v>
@@ -15073,8 +15111,8 @@
       <c r="K260" s="1" t="inlineStr">
         <is>
           <t>"natural = peak", 50
-"natural = hill", 438
-"place = locality", 386</t>
+"natural = hill", 439
+"place = locality", 387</t>
         </is>
       </c>
       <c r="L260" s="2" t="inlineStr">
@@ -15120,7 +15158,7 @@
         </is>
       </c>
       <c r="F261" t="n">
-        <v>21970</v>
+        <v>21641</v>
       </c>
       <c r="G261" s="12" t="n">
         <v>22178</v>
@@ -15144,8 +15182,8 @@
         <is>
           <t>"man_made = survey_point", 18
 "natural = peak", 252
-"place = locality", 314
-"natural = hill", 231</t>
+"place = locality", 331
+"natural = hill", 248</t>
         </is>
       </c>
       <c r="L261" s="17" t="inlineStr">
@@ -15191,7 +15229,7 @@
         </is>
       </c>
       <c r="F262" t="n">
-        <v>8444</v>
+        <v>9390</v>
       </c>
       <c r="G262" s="12" t="n">
         <v>8191</v>
@@ -15213,9 +15251,8 @@
       </c>
       <c r="K262" s="1" t="inlineStr">
         <is>
-          <t>"natural = heath", 58
-"natural = hill", 1013
-"place = locality", 1021</t>
+          <t>"natural = hill", 1471
+"place = locality", 1484</t>
         </is>
       </c>
       <c r="L262" s="17" t="inlineStr">
@@ -15261,7 +15298,7 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>9437</v>
+        <v>9906</v>
       </c>
       <c r="G263" s="12" t="n">
         <v>9146</v>
@@ -15283,8 +15320,8 @@
       </c>
       <c r="K263" s="1" t="inlineStr">
         <is>
-          <t>"natural = hill", 1046
-"place = locality", 747</t>
+          <t>"natural = hill", 1199
+"place = locality", 901</t>
         </is>
       </c>
       <c r="L263" s="17" t="inlineStr">
@@ -15325,7 +15362,7 @@
         </is>
       </c>
       <c r="F264" t="n">
-        <v>56165</v>
+        <v>57044</v>
       </c>
       <c r="G264" s="12" t="n">
         <v>57885</v>
@@ -15347,9 +15384,9 @@
       </c>
       <c r="K264" s="1" t="inlineStr">
         <is>
-          <t>"natural = hill", 3170
-"place = locality", 1866
-"natural = peak", 489
+          <t>"natural = hill", 3505
+"place = locality", 2200
+"natural = peak", 494
 "natural = ridge", 288</t>
         </is>
       </c>
@@ -15401,7 +15438,7 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>6909</v>
+        <v>6913</v>
       </c>
       <c r="G265" s="12" t="n">
         <v>6752</v>
@@ -15423,9 +15460,9 @@
       </c>
       <c r="K265" s="1" t="inlineStr">
         <is>
-          <t>"natural = hill", 42
-"natural = ridge", 231
-"place = locality", 152</t>
+          <t>"natural = hill", 68
+"natural = ridge", 238
+"place = locality", 186</t>
         </is>
       </c>
       <c r="L265" s="17" t="inlineStr">
@@ -15466,7 +15503,7 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>47844</v>
+        <v>46270</v>
       </c>
       <c r="G266" s="12" t="n">
         <v>48481</v>
@@ -15488,9 +15525,9 @@
       </c>
       <c r="K266" s="1" t="inlineStr">
         <is>
-          <t>"natural = peak", 144
-"natural = hill", 1718
-"place = locality", 1417</t>
+          <t>"natural = peak", 151
+"natural = hill", 1768
+"place = locality", 1472</t>
         </is>
       </c>
       <c r="L266" s="17" t="inlineStr">
@@ -15531,7 +15568,7 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>1804</v>
+        <v>1832</v>
       </c>
       <c r="G267" s="12" t="n">
         <v>1648</v>
@@ -15605,7 +15642,7 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>1184</v>
+        <v>1222</v>
       </c>
       <c r="G268" s="12" t="n">
         <v>1076</v>
@@ -15730,7 +15767,7 @@
         </is>
       </c>
       <c r="F271" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G271" s="12" t="n">
         <v>251</v>
@@ -15789,7 +15826,7 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>38650</v>
+        <v>39318</v>
       </c>
       <c r="G272" s="12" t="n">
         <v>38753</v>
@@ -15811,8 +15848,8 @@
       </c>
       <c r="K272" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 795
-"natural = valley", 1131</t>
+          <t>"place = locality", 1106
+"natural = valley", 1444</t>
         </is>
       </c>
       <c r="L272" s="17" t="inlineStr">
@@ -15853,7 +15890,7 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>6799</v>
+        <v>6380</v>
       </c>
       <c r="G273" s="12" t="n">
         <v>6491</v>
@@ -15875,8 +15912,8 @@
       </c>
       <c r="K273" s="1" t="inlineStr">
         <is>
-          <t>"natural = valley", 78
-"place = locality", 81</t>
+          <t>"natural = valley", 89
+"place = locality", 94</t>
         </is>
       </c>
       <c r="L273" s="17" t="inlineStr">
@@ -15917,7 +15954,7 @@
         </is>
       </c>
       <c r="F274" t="n">
-        <v>11073</v>
+        <v>11099</v>
       </c>
       <c r="G274" s="12" t="n">
         <v>11649</v>
@@ -15939,8 +15976,8 @@
       </c>
       <c r="K274" s="1" t="inlineStr">
         <is>
-          <t>"natural = valley", 126
-"place = locality", 109</t>
+          <t>"natural = valley", 148
+"place = locality", 131</t>
         </is>
       </c>
       <c r="L274" s="2" t="inlineStr">
@@ -15981,7 +16018,7 @@
         </is>
       </c>
       <c r="F275" t="n">
-        <v>2024</v>
+        <v>1905</v>
       </c>
       <c r="G275" s="12" t="n">
         <v>1747</v>
@@ -16040,7 +16077,7 @@
         </is>
       </c>
       <c r="F276" t="n">
-        <v>3250</v>
+        <v>3308</v>
       </c>
       <c r="G276" s="12" t="n">
         <v>2948</v>
@@ -16062,8 +16099,8 @@
       </c>
       <c r="K276" s="1" t="inlineStr">
         <is>
-          <t>"natural = valley", 53
-"place = locality", 42
+          <t>"natural = valley", 65
+"place = locality", 54
 "natural = wetland", 3
 "wetland = bog", 2</t>
         </is>
@@ -16111,7 +16148,7 @@
         </is>
       </c>
       <c r="F277" t="n">
-        <v>404</v>
+        <v>428</v>
       </c>
       <c r="G277" s="12" t="n">
         <v>340</v>
@@ -16133,8 +16170,8 @@
       </c>
       <c r="K277" s="1" t="inlineStr">
         <is>
-          <t>"natural = valley", 20
-"place = locality", 20</t>
+          <t>"natural = valley", 33
+"place = locality", 33</t>
         </is>
       </c>
       <c r="L277" s="17" t="inlineStr">
@@ -16208,7 +16245,7 @@
         </is>
       </c>
       <c r="F279" t="n">
-        <v>12646</v>
+        <v>12675</v>
       </c>
       <c r="G279" s="12" t="n">
         <v>11974</v>
@@ -16230,8 +16267,8 @@
       </c>
       <c r="K279" s="1" t="inlineStr">
         <is>
-          <t>"natural = slope", 292
-"place = locality", 302</t>
+          <t>"natural = slope", 324
+"place = locality", 334</t>
         </is>
       </c>
       <c r="L279" s="17" t="inlineStr">
@@ -16272,7 +16309,7 @@
         </is>
       </c>
       <c r="F280" t="n">
-        <v>33347</v>
+        <v>33657</v>
       </c>
       <c r="G280" s="12" t="n">
         <v>32819</v>
@@ -16294,8 +16331,8 @@
       </c>
       <c r="K280" s="1" t="inlineStr">
         <is>
-          <t>"natural = slope", 815
-"place = locality", 830</t>
+          <t>"natural = slope", 864
+"place = locality", 879</t>
         </is>
       </c>
       <c r="L280" s="17" t="inlineStr">
@@ -16336,7 +16373,7 @@
         </is>
       </c>
       <c r="F281" t="n">
-        <v>1467</v>
+        <v>1573</v>
       </c>
       <c r="G281" s="12" t="n">
         <v>1437</v>
@@ -16358,7 +16395,7 @@
       </c>
       <c r="K281" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 15</t>
+          <t>"place = locality", 24</t>
         </is>
       </c>
       <c r="M281" s="12" t="inlineStr">
@@ -16427,7 +16464,7 @@
         </is>
       </c>
       <c r="F283" t="n">
-        <v>3067</v>
+        <v>3161</v>
       </c>
       <c r="G283" s="12" t="n">
         <v>2726</v>
@@ -16449,7 +16486,7 @@
       </c>
       <c r="K283" s="1" t="inlineStr">
         <is>
-          <t>"natural = cliff", 150</t>
+          <t>"natural = cliff", 162</t>
         </is>
       </c>
       <c r="L283" s="17" t="inlineStr">
@@ -16486,7 +16523,7 @@
         </is>
       </c>
       <c r="F284" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G284" s="12" t="n">
         <v>513</v>
@@ -16508,7 +16545,7 @@
       </c>
       <c r="K284" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 6</t>
+          <t>"place = locality", 7</t>
         </is>
       </c>
       <c r="L284" s="2" t="n"/>
@@ -16545,7 +16582,7 @@
         </is>
       </c>
       <c r="F285" t="n">
-        <v>3449</v>
+        <v>3267</v>
       </c>
       <c r="G285" s="12" t="n">
         <v>2244</v>
@@ -16567,7 +16604,7 @@
       </c>
       <c r="K285" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 131</t>
+          <t>"place = locality", 132</t>
         </is>
       </c>
       <c r="M285" s="12" t="inlineStr">
@@ -16603,7 +16640,7 @@
         </is>
       </c>
       <c r="F286" t="n">
-        <v>6491</v>
+        <v>6565</v>
       </c>
       <c r="G286" s="12" t="n">
         <v>6057</v>
@@ -16625,7 +16662,7 @@
       </c>
       <c r="K286" s="1" t="inlineStr">
         <is>
-          <t>"place = locality", 104</t>
+          <t>"place = locality", 131</t>
         </is>
       </c>
       <c r="M286" s="12" t="inlineStr">
@@ -16815,7 +16852,7 @@
         </is>
       </c>
       <c r="F290" t="n">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="G290" s="12" t="n">
         <v>337</v>
@@ -16879,7 +16916,7 @@
         </is>
       </c>
       <c r="F291" t="n">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="G291" s="12" t="n">
         <v>279</v>
@@ -16899,7 +16936,12 @@
           <t>Høyereliggende, større område uten skog med lave terrengvariasjoner  innenfor området. Eks. Valdresflye, Hardangervidda, Finnmarksvidda, Laksefjordvidda</t>
         </is>
       </c>
-      <c r="K291" s="1" t="inlineStr"/>
+      <c r="K291" s="1" t="inlineStr">
+        <is>
+          <t>"natural = mountain_range", 2
+"note = Please refine boundary based on local knowledge", 2</t>
+        </is>
+      </c>
       <c r="L291" s="17" t="inlineStr">
         <is>
           <t>natural=plateau</t>
@@ -16933,7 +16975,7 @@
         </is>
       </c>
       <c r="F292" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G292" s="12" t="n">
         <v>44</v>
@@ -16957,7 +16999,7 @@
         <is>
           <t>"place = farm", 2
 "place = isolated_dwelling", 2
-"place = locality", 8</t>
+"place = locality", 16</t>
         </is>
       </c>
       <c r="L292" s="17" t="inlineStr">

</xml_diff>